<commit_message>
VRT Project updated with Policy Test Set Data & Test xml updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/PolicyTestdata.xlsx
+++ b/src/test/resources/TestData/PolicyTestdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\git\VRT\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\VRT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E09620E-C826-42EF-A8C7-4C7E5A97F21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6A9D61-2227-4EAE-B665-23212050E438}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="886" firstSheet="34" activeTab="44" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11070" tabRatio="886" firstSheet="22" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Policies003" sheetId="1" r:id="rId1"/>
@@ -1780,12 +1780,6 @@
     <t>32</t>
   </si>
   <si>
-    <t>PLT008b1</t>
-  </si>
-  <si>
-    <t>8b1</t>
-  </si>
-  <si>
     <t>15b1</t>
   </si>
   <si>
@@ -1816,12 +1810,6 @@
     <t>p023</t>
   </si>
   <si>
-    <t>PLT008d1</t>
-  </si>
-  <si>
-    <t>8d1</t>
-  </si>
-  <si>
     <t>730</t>
   </si>
   <si>
@@ -1831,12 +1819,6 @@
     <t>15ba11</t>
   </si>
   <si>
-    <t>PLT008E1</t>
-  </si>
-  <si>
-    <t>8E1</t>
-  </si>
-  <si>
     <t>124456</t>
   </si>
   <si>
@@ -1850,6 +1832,24 @@
   </si>
   <si>
     <t>12PLB</t>
+  </si>
+  <si>
+    <t>PLT008a</t>
+  </si>
+  <si>
+    <t>8a</t>
+  </si>
+  <si>
+    <t>PLT008d</t>
+  </si>
+  <si>
+    <t>8d</t>
+  </si>
+  <si>
+    <t>PLT008E</t>
+  </si>
+  <si>
+    <t>8E</t>
   </si>
 </sst>
 </file>
@@ -2307,17 +2307,17 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
@@ -2383,16 +2383,16 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -2458,16 +2458,16 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" customWidth="1"/>
-    <col min="6" max="6" width="28.109375" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
@@ -2533,17 +2533,17 @@
       <selection activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>34</v>
       </c>
@@ -2605,17 +2605,17 @@
       <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" customWidth="1"/>
-    <col min="8" max="8" width="62.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="62.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>41</v>
       </c>
@@ -2683,17 +2683,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="92" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>44</v>
       </c>
@@ -2761,17 +2761,17 @@
       <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" customWidth="1"/>
-    <col min="8" max="8" width="72.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="72.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>56</v>
       </c>
@@ -2839,18 +2839,18 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="73.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="73.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>57</v>
       </c>
@@ -2918,16 +2918,16 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="24.109375" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="3" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
-    <col min="7" max="7" width="33.109375" customWidth="1"/>
-    <col min="8" max="8" width="82.5546875" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" customWidth="1"/>
+    <col min="8" max="8" width="82.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>58</v>
       </c>
@@ -2995,17 +2995,17 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
-    <col min="4" max="5" width="23.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="5" width="23.5703125" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" customWidth="1"/>
-    <col min="8" max="8" width="73.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="73.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>59</v>
       </c>
@@ -3073,17 +3073,17 @@
       <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.5546875" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" customWidth="1"/>
-    <col min="8" max="8" width="59.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="59.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>60</v>
       </c>
@@ -3151,13 +3151,13 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -3223,17 +3223,17 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="23.88671875" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="63.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="63.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>62</v>
       </c>
@@ -3301,17 +3301,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" customWidth="1"/>
-    <col min="8" max="8" width="62.5546875" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="62.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>67</v>
       </c>
@@ -3379,17 +3379,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="27.109375" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" customWidth="1"/>
-    <col min="8" max="8" width="55.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="55.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>163</v>
       </c>
@@ -3457,17 +3457,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>165</v>
       </c>
@@ -3531,21 +3531,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E336E99-E12B-4B5D-8E02-D35BF6E90D3C}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" customWidth="1"/>
-    <col min="7" max="7" width="50.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="50.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3571,12 +3571,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>105</v>
+        <v>186</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>6</v>
@@ -3611,21 +3611,21 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" customWidth="1"/>
-    <col min="7" max="7" width="25.88671875" customWidth="1"/>
-    <col min="8" max="8" width="48.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
+    <col min="8" max="8" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3651,12 +3651,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>167</v>
+        <v>106</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>168</v>
+        <v>105</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>114</v>
@@ -3694,17 +3694,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3730,7 +3730,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>109</v>
       </c>
@@ -3769,23 +3769,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D01A18E-360B-4012-81C6-2FE21FE6E96A}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" customWidth="1"/>
-    <col min="6" max="6" width="28.44140625" customWidth="1"/>
-    <col min="7" max="7" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.109375" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3811,12 +3811,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>115</v>
@@ -3834,7 +3834,7 @@
         <v>72</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -3850,23 +3850,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0D683C-79DC-4FEE-BEFB-15848DFF7B1E}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1"/>
-    <col min="7" max="7" width="45.44140625" customWidth="1"/>
-    <col min="8" max="8" width="45.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="45.42578125" customWidth="1"/>
+    <col min="8" max="8" width="45.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3892,12 +3892,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>117</v>
@@ -3932,16 +3932,16 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>70</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>120</v>
       </c>
@@ -3971,17 +3971,17 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -4047,19 +4047,19 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4085,15 +4085,15 @@
         <v>104</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>116</v>
@@ -4105,7 +4105,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>72</v>
@@ -4114,7 +4114,7 @@
         <v>84</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -4134,17 +4134,17 @@
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
-    <col min="7" max="7" width="43.5546875" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="43.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>125</v>
       </c>
@@ -4213,12 +4213,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="95.5546875" customWidth="1"/>
+    <col min="1" max="1" width="95.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>70</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>126</v>
       </c>
@@ -4248,17 +4248,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" customWidth="1"/>
-    <col min="7" max="7" width="55.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="55.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4281,7 +4281,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>130</v>
       </c>
@@ -4321,18 +4321,18 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="7" max="7" width="57.5546875" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="57.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4355,12 +4355,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>122</v>
@@ -4395,15 +4395,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" customWidth="1"/>
-    <col min="7" max="7" width="58.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4426,12 +4426,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>122</v>
@@ -4466,12 +4466,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4491,12 +4491,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>122</v>
@@ -4528,15 +4528,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4556,12 +4556,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>122</v>
@@ -4593,15 +4593,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
-    <col min="5" max="5" width="19.88671875" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4621,12 +4621,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>122</v>
@@ -4658,16 +4658,16 @@
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.88671875" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="26.109375" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>131</v>
       </c>
@@ -4724,17 +4724,17 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -4800,15 +4800,15 @@
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>133</v>
       </c>
@@ -4865,17 +4865,17 @@
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>140</v>
       </c>
@@ -4932,15 +4932,15 @@
       <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>141</v>
       </c>
@@ -4997,15 +4997,15 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>144</v>
       </c>
@@ -5062,16 +5062,16 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="45.5546875" customWidth="1"/>
+    <col min="7" max="7" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>146</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>149</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>160</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>159</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>158</v>
       </c>
@@ -5229,20 +5229,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9984D82-920C-461A-98FF-A41A7669EA6A}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -5259,12 +5259,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>122</v>
@@ -5292,17 +5292,17 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5328,7 +5328,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -5368,18 +5368,18 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5405,7 +5405,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -5445,16 +5445,16 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
@@ -5520,16 +5520,16 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -5595,16 +5595,16 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>30</v>
       </c>

</xml_diff>